<commit_message>
added mango and shaga testnet
</commit_message>
<xml_diff>
--- a/AIRDROP.xlsx
+++ b/AIRDROP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80373A3B-034D-452F-A4FF-E0E042FB577B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0252F666-30E0-47E0-B0E0-2B55C9D5353C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
-  <si>
-    <t>NO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="112">
   <si>
     <t>NAME</t>
   </si>
@@ -335,6 +332,30 @@
   </si>
   <si>
     <t>CHAIN OPERA</t>
+  </si>
+  <si>
+    <t>SHAGA GLOB</t>
+  </si>
+  <si>
+    <t>https://glob.shaga.xyz/?r=Bdgdwjwdtb</t>
+  </si>
+  <si>
+    <t>CHAIN/DEPIN</t>
+  </si>
+  <si>
+    <t>https://task.testnet.mangonetwork.io/?invite=FHKOiL</t>
+  </si>
+  <si>
+    <t>MANGO NETWORK</t>
+  </si>
+  <si>
+    <t>https://t.me/KeoAirDropFreeNe/323/37670</t>
+  </si>
+  <si>
+    <t>SINGULARITY FINANCE</t>
+  </si>
+  <si>
+    <t>FINANCE/TESTNET</t>
   </si>
 </sst>
 </file>
@@ -816,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,20 +851,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -851,16 +870,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="E2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -868,16 +887,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -885,16 +904,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -902,16 +921,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -919,16 +938,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -936,16 +955,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -953,16 +972,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,16 +989,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -987,16 +1006,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1004,16 +1023,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1021,16 +1040,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="E12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1038,16 +1057,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1055,16 +1074,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>60</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1072,16 +1091,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1089,16 +1108,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1106,16 +1125,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1123,16 +1142,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1140,16 +1159,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1157,16 +1176,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1174,16 +1193,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="E21" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1191,16 +1210,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>58</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1208,16 +1227,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="D23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1225,16 +1244,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1242,16 +1261,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1259,16 +1278,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1276,16 +1295,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1293,16 +1312,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="E28" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1310,16 +1329,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="D29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="E29" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1327,16 +1346,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1344,16 +1363,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1361,16 +1380,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1378,16 +1397,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1395,16 +1414,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1412,16 +1431,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1429,16 +1448,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1446,16 +1465,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="E37" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1463,16 +1482,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1480,16 +1499,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="D39" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E39" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1497,16 +1516,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="D40" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="E40" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1514,16 +1533,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1531,44 +1550,68 @@
         <v>41</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="6"/>
+      <c r="B43" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="6"/>
+      <c r="B44" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="6"/>
+      <c r="B45" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
@@ -2158,8 +2201,9 @@
     <hyperlink ref="C20" r:id="rId28" xr:uid="{E7616A7A-28A4-453B-931D-92984C36B89E}"/>
     <hyperlink ref="C16" r:id="rId29" xr:uid="{9C2F4246-FA24-4317-9051-3D008DA7AF0A}"/>
     <hyperlink ref="C24" r:id="rId30" xr:uid="{0C4EF850-072D-4ABA-8411-F542B8A43F7E}"/>
+    <hyperlink ref="C44" r:id="rId31" xr:uid="{115F76D7-8106-401F-8699-705C809125CA}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>